<commit_message>
Actualizando matriz de trazabilidad
</commit_message>
<xml_diff>
--- a/METODOLOGIA RUP/PROYECTO STD/02 REQUISITOS/STD_MATR_TRAZ.xlsx
+++ b/METODOLOGIA RUP/PROYECTO STD/02 REQUISITOS/STD_MATR_TRAZ.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
   <si>
     <t>Registrar Informe</t>
   </si>
@@ -111,9 +111,6 @@
     <t>Actualizacion de datos de usuarios</t>
   </si>
   <si>
-    <t>Consultar Requisitos</t>
-  </si>
-  <si>
     <t>Registrar tramite</t>
   </si>
   <si>
@@ -138,9 +135,6 @@
     <t>Gestionar usuarios</t>
   </si>
   <si>
-    <t>CASO DE USO</t>
-  </si>
-  <si>
     <t xml:space="preserve"> MATRIZ DE TRAZABILIDAD</t>
   </si>
   <si>
@@ -184,16 +178,13 @@
   </si>
   <si>
     <t>CU-10</t>
-  </si>
-  <si>
-    <t>CU-11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -272,7 +263,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -318,19 +309,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -358,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -385,9 +363,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -404,9 +379,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -498,6 +470,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -532,6 +505,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -707,363 +681,360 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" style="2" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="53.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="13" width="4.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.42578125" style="2" customWidth="1"/>
-    <col min="16" max="238" width="17.140625" style="2"/>
-    <col min="239" max="239" width="8" style="2" customWidth="1"/>
-    <col min="240" max="240" width="10.85546875" style="2" customWidth="1"/>
-    <col min="241" max="241" width="69.7109375" style="2" customWidth="1"/>
-    <col min="242" max="271" width="4.42578125" style="2" customWidth="1"/>
-    <col min="272" max="494" width="17.140625" style="2"/>
-    <col min="495" max="495" width="8" style="2" customWidth="1"/>
-    <col min="496" max="496" width="10.85546875" style="2" customWidth="1"/>
-    <col min="497" max="497" width="69.7109375" style="2" customWidth="1"/>
-    <col min="498" max="527" width="4.42578125" style="2" customWidth="1"/>
-    <col min="528" max="750" width="17.140625" style="2"/>
-    <col min="751" max="751" width="8" style="2" customWidth="1"/>
-    <col min="752" max="752" width="10.85546875" style="2" customWidth="1"/>
-    <col min="753" max="753" width="69.7109375" style="2" customWidth="1"/>
-    <col min="754" max="783" width="4.42578125" style="2" customWidth="1"/>
-    <col min="784" max="1006" width="17.140625" style="2"/>
-    <col min="1007" max="1007" width="8" style="2" customWidth="1"/>
-    <col min="1008" max="1008" width="10.85546875" style="2" customWidth="1"/>
-    <col min="1009" max="1009" width="69.7109375" style="2" customWidth="1"/>
-    <col min="1010" max="1039" width="4.42578125" style="2" customWidth="1"/>
-    <col min="1040" max="1262" width="17.140625" style="2"/>
-    <col min="1263" max="1263" width="8" style="2" customWidth="1"/>
-    <col min="1264" max="1264" width="10.85546875" style="2" customWidth="1"/>
-    <col min="1265" max="1265" width="69.7109375" style="2" customWidth="1"/>
-    <col min="1266" max="1295" width="4.42578125" style="2" customWidth="1"/>
-    <col min="1296" max="1518" width="17.140625" style="2"/>
-    <col min="1519" max="1519" width="8" style="2" customWidth="1"/>
-    <col min="1520" max="1520" width="10.85546875" style="2" customWidth="1"/>
-    <col min="1521" max="1521" width="69.7109375" style="2" customWidth="1"/>
-    <col min="1522" max="1551" width="4.42578125" style="2" customWidth="1"/>
-    <col min="1552" max="1774" width="17.140625" style="2"/>
-    <col min="1775" max="1775" width="8" style="2" customWidth="1"/>
-    <col min="1776" max="1776" width="10.85546875" style="2" customWidth="1"/>
-    <col min="1777" max="1777" width="69.7109375" style="2" customWidth="1"/>
-    <col min="1778" max="1807" width="4.42578125" style="2" customWidth="1"/>
-    <col min="1808" max="2030" width="17.140625" style="2"/>
-    <col min="2031" max="2031" width="8" style="2" customWidth="1"/>
-    <col min="2032" max="2032" width="10.85546875" style="2" customWidth="1"/>
-    <col min="2033" max="2033" width="69.7109375" style="2" customWidth="1"/>
-    <col min="2034" max="2063" width="4.42578125" style="2" customWidth="1"/>
-    <col min="2064" max="2286" width="17.140625" style="2"/>
-    <col min="2287" max="2287" width="8" style="2" customWidth="1"/>
-    <col min="2288" max="2288" width="10.85546875" style="2" customWidth="1"/>
-    <col min="2289" max="2289" width="69.7109375" style="2" customWidth="1"/>
-    <col min="2290" max="2319" width="4.42578125" style="2" customWidth="1"/>
-    <col min="2320" max="2542" width="17.140625" style="2"/>
-    <col min="2543" max="2543" width="8" style="2" customWidth="1"/>
-    <col min="2544" max="2544" width="10.85546875" style="2" customWidth="1"/>
-    <col min="2545" max="2545" width="69.7109375" style="2" customWidth="1"/>
-    <col min="2546" max="2575" width="4.42578125" style="2" customWidth="1"/>
-    <col min="2576" max="2798" width="17.140625" style="2"/>
-    <col min="2799" max="2799" width="8" style="2" customWidth="1"/>
-    <col min="2800" max="2800" width="10.85546875" style="2" customWidth="1"/>
-    <col min="2801" max="2801" width="69.7109375" style="2" customWidth="1"/>
-    <col min="2802" max="2831" width="4.42578125" style="2" customWidth="1"/>
-    <col min="2832" max="3054" width="17.140625" style="2"/>
-    <col min="3055" max="3055" width="8" style="2" customWidth="1"/>
-    <col min="3056" max="3056" width="10.85546875" style="2" customWidth="1"/>
-    <col min="3057" max="3057" width="69.7109375" style="2" customWidth="1"/>
-    <col min="3058" max="3087" width="4.42578125" style="2" customWidth="1"/>
-    <col min="3088" max="3310" width="17.140625" style="2"/>
-    <col min="3311" max="3311" width="8" style="2" customWidth="1"/>
-    <col min="3312" max="3312" width="10.85546875" style="2" customWidth="1"/>
-    <col min="3313" max="3313" width="69.7109375" style="2" customWidth="1"/>
-    <col min="3314" max="3343" width="4.42578125" style="2" customWidth="1"/>
-    <col min="3344" max="3566" width="17.140625" style="2"/>
-    <col min="3567" max="3567" width="8" style="2" customWidth="1"/>
-    <col min="3568" max="3568" width="10.85546875" style="2" customWidth="1"/>
-    <col min="3569" max="3569" width="69.7109375" style="2" customWidth="1"/>
-    <col min="3570" max="3599" width="4.42578125" style="2" customWidth="1"/>
-    <col min="3600" max="3822" width="17.140625" style="2"/>
-    <col min="3823" max="3823" width="8" style="2" customWidth="1"/>
-    <col min="3824" max="3824" width="10.85546875" style="2" customWidth="1"/>
-    <col min="3825" max="3825" width="69.7109375" style="2" customWidth="1"/>
-    <col min="3826" max="3855" width="4.42578125" style="2" customWidth="1"/>
-    <col min="3856" max="4078" width="17.140625" style="2"/>
-    <col min="4079" max="4079" width="8" style="2" customWidth="1"/>
-    <col min="4080" max="4080" width="10.85546875" style="2" customWidth="1"/>
-    <col min="4081" max="4081" width="69.7109375" style="2" customWidth="1"/>
-    <col min="4082" max="4111" width="4.42578125" style="2" customWidth="1"/>
-    <col min="4112" max="4334" width="17.140625" style="2"/>
-    <col min="4335" max="4335" width="8" style="2" customWidth="1"/>
-    <col min="4336" max="4336" width="10.85546875" style="2" customWidth="1"/>
-    <col min="4337" max="4337" width="69.7109375" style="2" customWidth="1"/>
-    <col min="4338" max="4367" width="4.42578125" style="2" customWidth="1"/>
-    <col min="4368" max="4590" width="17.140625" style="2"/>
-    <col min="4591" max="4591" width="8" style="2" customWidth="1"/>
-    <col min="4592" max="4592" width="10.85546875" style="2" customWidth="1"/>
-    <col min="4593" max="4593" width="69.7109375" style="2" customWidth="1"/>
-    <col min="4594" max="4623" width="4.42578125" style="2" customWidth="1"/>
-    <col min="4624" max="4846" width="17.140625" style="2"/>
-    <col min="4847" max="4847" width="8" style="2" customWidth="1"/>
-    <col min="4848" max="4848" width="10.85546875" style="2" customWidth="1"/>
-    <col min="4849" max="4849" width="69.7109375" style="2" customWidth="1"/>
-    <col min="4850" max="4879" width="4.42578125" style="2" customWidth="1"/>
-    <col min="4880" max="5102" width="17.140625" style="2"/>
-    <col min="5103" max="5103" width="8" style="2" customWidth="1"/>
-    <col min="5104" max="5104" width="10.85546875" style="2" customWidth="1"/>
-    <col min="5105" max="5105" width="69.7109375" style="2" customWidth="1"/>
-    <col min="5106" max="5135" width="4.42578125" style="2" customWidth="1"/>
-    <col min="5136" max="5358" width="17.140625" style="2"/>
-    <col min="5359" max="5359" width="8" style="2" customWidth="1"/>
-    <col min="5360" max="5360" width="10.85546875" style="2" customWidth="1"/>
-    <col min="5361" max="5361" width="69.7109375" style="2" customWidth="1"/>
-    <col min="5362" max="5391" width="4.42578125" style="2" customWidth="1"/>
-    <col min="5392" max="5614" width="17.140625" style="2"/>
-    <col min="5615" max="5615" width="8" style="2" customWidth="1"/>
-    <col min="5616" max="5616" width="10.85546875" style="2" customWidth="1"/>
-    <col min="5617" max="5617" width="69.7109375" style="2" customWidth="1"/>
-    <col min="5618" max="5647" width="4.42578125" style="2" customWidth="1"/>
-    <col min="5648" max="5870" width="17.140625" style="2"/>
-    <col min="5871" max="5871" width="8" style="2" customWidth="1"/>
-    <col min="5872" max="5872" width="10.85546875" style="2" customWidth="1"/>
-    <col min="5873" max="5873" width="69.7109375" style="2" customWidth="1"/>
-    <col min="5874" max="5903" width="4.42578125" style="2" customWidth="1"/>
-    <col min="5904" max="6126" width="17.140625" style="2"/>
-    <col min="6127" max="6127" width="8" style="2" customWidth="1"/>
-    <col min="6128" max="6128" width="10.85546875" style="2" customWidth="1"/>
-    <col min="6129" max="6129" width="69.7109375" style="2" customWidth="1"/>
-    <col min="6130" max="6159" width="4.42578125" style="2" customWidth="1"/>
-    <col min="6160" max="6382" width="17.140625" style="2"/>
-    <col min="6383" max="6383" width="8" style="2" customWidth="1"/>
-    <col min="6384" max="6384" width="10.85546875" style="2" customWidth="1"/>
-    <col min="6385" max="6385" width="69.7109375" style="2" customWidth="1"/>
-    <col min="6386" max="6415" width="4.42578125" style="2" customWidth="1"/>
-    <col min="6416" max="6638" width="17.140625" style="2"/>
-    <col min="6639" max="6639" width="8" style="2" customWidth="1"/>
-    <col min="6640" max="6640" width="10.85546875" style="2" customWidth="1"/>
-    <col min="6641" max="6641" width="69.7109375" style="2" customWidth="1"/>
-    <col min="6642" max="6671" width="4.42578125" style="2" customWidth="1"/>
-    <col min="6672" max="6894" width="17.140625" style="2"/>
-    <col min="6895" max="6895" width="8" style="2" customWidth="1"/>
-    <col min="6896" max="6896" width="10.85546875" style="2" customWidth="1"/>
-    <col min="6897" max="6897" width="69.7109375" style="2" customWidth="1"/>
-    <col min="6898" max="6927" width="4.42578125" style="2" customWidth="1"/>
-    <col min="6928" max="7150" width="17.140625" style="2"/>
-    <col min="7151" max="7151" width="8" style="2" customWidth="1"/>
-    <col min="7152" max="7152" width="10.85546875" style="2" customWidth="1"/>
-    <col min="7153" max="7153" width="69.7109375" style="2" customWidth="1"/>
-    <col min="7154" max="7183" width="4.42578125" style="2" customWidth="1"/>
-    <col min="7184" max="7406" width="17.140625" style="2"/>
-    <col min="7407" max="7407" width="8" style="2" customWidth="1"/>
-    <col min="7408" max="7408" width="10.85546875" style="2" customWidth="1"/>
-    <col min="7409" max="7409" width="69.7109375" style="2" customWidth="1"/>
-    <col min="7410" max="7439" width="4.42578125" style="2" customWidth="1"/>
-    <col min="7440" max="7662" width="17.140625" style="2"/>
-    <col min="7663" max="7663" width="8" style="2" customWidth="1"/>
-    <col min="7664" max="7664" width="10.85546875" style="2" customWidth="1"/>
-    <col min="7665" max="7665" width="69.7109375" style="2" customWidth="1"/>
-    <col min="7666" max="7695" width="4.42578125" style="2" customWidth="1"/>
-    <col min="7696" max="7918" width="17.140625" style="2"/>
-    <col min="7919" max="7919" width="8" style="2" customWidth="1"/>
-    <col min="7920" max="7920" width="10.85546875" style="2" customWidth="1"/>
-    <col min="7921" max="7921" width="69.7109375" style="2" customWidth="1"/>
-    <col min="7922" max="7951" width="4.42578125" style="2" customWidth="1"/>
-    <col min="7952" max="8174" width="17.140625" style="2"/>
-    <col min="8175" max="8175" width="8" style="2" customWidth="1"/>
-    <col min="8176" max="8176" width="10.85546875" style="2" customWidth="1"/>
-    <col min="8177" max="8177" width="69.7109375" style="2" customWidth="1"/>
-    <col min="8178" max="8207" width="4.42578125" style="2" customWidth="1"/>
-    <col min="8208" max="8430" width="17.140625" style="2"/>
-    <col min="8431" max="8431" width="8" style="2" customWidth="1"/>
-    <col min="8432" max="8432" width="10.85546875" style="2" customWidth="1"/>
-    <col min="8433" max="8433" width="69.7109375" style="2" customWidth="1"/>
-    <col min="8434" max="8463" width="4.42578125" style="2" customWidth="1"/>
-    <col min="8464" max="8686" width="17.140625" style="2"/>
-    <col min="8687" max="8687" width="8" style="2" customWidth="1"/>
-    <col min="8688" max="8688" width="10.85546875" style="2" customWidth="1"/>
-    <col min="8689" max="8689" width="69.7109375" style="2" customWidth="1"/>
-    <col min="8690" max="8719" width="4.42578125" style="2" customWidth="1"/>
-    <col min="8720" max="8942" width="17.140625" style="2"/>
-    <col min="8943" max="8943" width="8" style="2" customWidth="1"/>
-    <col min="8944" max="8944" width="10.85546875" style="2" customWidth="1"/>
-    <col min="8945" max="8945" width="69.7109375" style="2" customWidth="1"/>
-    <col min="8946" max="8975" width="4.42578125" style="2" customWidth="1"/>
-    <col min="8976" max="9198" width="17.140625" style="2"/>
-    <col min="9199" max="9199" width="8" style="2" customWidth="1"/>
-    <col min="9200" max="9200" width="10.85546875" style="2" customWidth="1"/>
-    <col min="9201" max="9201" width="69.7109375" style="2" customWidth="1"/>
-    <col min="9202" max="9231" width="4.42578125" style="2" customWidth="1"/>
-    <col min="9232" max="9454" width="17.140625" style="2"/>
-    <col min="9455" max="9455" width="8" style="2" customWidth="1"/>
-    <col min="9456" max="9456" width="10.85546875" style="2" customWidth="1"/>
-    <col min="9457" max="9457" width="69.7109375" style="2" customWidth="1"/>
-    <col min="9458" max="9487" width="4.42578125" style="2" customWidth="1"/>
-    <col min="9488" max="9710" width="17.140625" style="2"/>
-    <col min="9711" max="9711" width="8" style="2" customWidth="1"/>
-    <col min="9712" max="9712" width="10.85546875" style="2" customWidth="1"/>
-    <col min="9713" max="9713" width="69.7109375" style="2" customWidth="1"/>
-    <col min="9714" max="9743" width="4.42578125" style="2" customWidth="1"/>
-    <col min="9744" max="9966" width="17.140625" style="2"/>
-    <col min="9967" max="9967" width="8" style="2" customWidth="1"/>
-    <col min="9968" max="9968" width="10.85546875" style="2" customWidth="1"/>
-    <col min="9969" max="9969" width="69.7109375" style="2" customWidth="1"/>
-    <col min="9970" max="9999" width="4.42578125" style="2" customWidth="1"/>
-    <col min="10000" max="10222" width="17.140625" style="2"/>
-    <col min="10223" max="10223" width="8" style="2" customWidth="1"/>
-    <col min="10224" max="10224" width="10.85546875" style="2" customWidth="1"/>
-    <col min="10225" max="10225" width="69.7109375" style="2" customWidth="1"/>
-    <col min="10226" max="10255" width="4.42578125" style="2" customWidth="1"/>
-    <col min="10256" max="10478" width="17.140625" style="2"/>
-    <col min="10479" max="10479" width="8" style="2" customWidth="1"/>
-    <col min="10480" max="10480" width="10.85546875" style="2" customWidth="1"/>
-    <col min="10481" max="10481" width="69.7109375" style="2" customWidth="1"/>
-    <col min="10482" max="10511" width="4.42578125" style="2" customWidth="1"/>
-    <col min="10512" max="10734" width="17.140625" style="2"/>
-    <col min="10735" max="10735" width="8" style="2" customWidth="1"/>
-    <col min="10736" max="10736" width="10.85546875" style="2" customWidth="1"/>
-    <col min="10737" max="10737" width="69.7109375" style="2" customWidth="1"/>
-    <col min="10738" max="10767" width="4.42578125" style="2" customWidth="1"/>
-    <col min="10768" max="10990" width="17.140625" style="2"/>
-    <col min="10991" max="10991" width="8" style="2" customWidth="1"/>
-    <col min="10992" max="10992" width="10.85546875" style="2" customWidth="1"/>
-    <col min="10993" max="10993" width="69.7109375" style="2" customWidth="1"/>
-    <col min="10994" max="11023" width="4.42578125" style="2" customWidth="1"/>
-    <col min="11024" max="11246" width="17.140625" style="2"/>
-    <col min="11247" max="11247" width="8" style="2" customWidth="1"/>
-    <col min="11248" max="11248" width="10.85546875" style="2" customWidth="1"/>
-    <col min="11249" max="11249" width="69.7109375" style="2" customWidth="1"/>
-    <col min="11250" max="11279" width="4.42578125" style="2" customWidth="1"/>
-    <col min="11280" max="11502" width="17.140625" style="2"/>
-    <col min="11503" max="11503" width="8" style="2" customWidth="1"/>
-    <col min="11504" max="11504" width="10.85546875" style="2" customWidth="1"/>
-    <col min="11505" max="11505" width="69.7109375" style="2" customWidth="1"/>
-    <col min="11506" max="11535" width="4.42578125" style="2" customWidth="1"/>
-    <col min="11536" max="11758" width="17.140625" style="2"/>
-    <col min="11759" max="11759" width="8" style="2" customWidth="1"/>
-    <col min="11760" max="11760" width="10.85546875" style="2" customWidth="1"/>
-    <col min="11761" max="11761" width="69.7109375" style="2" customWidth="1"/>
-    <col min="11762" max="11791" width="4.42578125" style="2" customWidth="1"/>
-    <col min="11792" max="12014" width="17.140625" style="2"/>
-    <col min="12015" max="12015" width="8" style="2" customWidth="1"/>
-    <col min="12016" max="12016" width="10.85546875" style="2" customWidth="1"/>
-    <col min="12017" max="12017" width="69.7109375" style="2" customWidth="1"/>
-    <col min="12018" max="12047" width="4.42578125" style="2" customWidth="1"/>
-    <col min="12048" max="12270" width="17.140625" style="2"/>
-    <col min="12271" max="12271" width="8" style="2" customWidth="1"/>
-    <col min="12272" max="12272" width="10.85546875" style="2" customWidth="1"/>
-    <col min="12273" max="12273" width="69.7109375" style="2" customWidth="1"/>
-    <col min="12274" max="12303" width="4.42578125" style="2" customWidth="1"/>
-    <col min="12304" max="12526" width="17.140625" style="2"/>
-    <col min="12527" max="12527" width="8" style="2" customWidth="1"/>
-    <col min="12528" max="12528" width="10.85546875" style="2" customWidth="1"/>
-    <col min="12529" max="12529" width="69.7109375" style="2" customWidth="1"/>
-    <col min="12530" max="12559" width="4.42578125" style="2" customWidth="1"/>
-    <col min="12560" max="12782" width="17.140625" style="2"/>
-    <col min="12783" max="12783" width="8" style="2" customWidth="1"/>
-    <col min="12784" max="12784" width="10.85546875" style="2" customWidth="1"/>
-    <col min="12785" max="12785" width="69.7109375" style="2" customWidth="1"/>
-    <col min="12786" max="12815" width="4.42578125" style="2" customWidth="1"/>
-    <col min="12816" max="13038" width="17.140625" style="2"/>
-    <col min="13039" max="13039" width="8" style="2" customWidth="1"/>
-    <col min="13040" max="13040" width="10.85546875" style="2" customWidth="1"/>
-    <col min="13041" max="13041" width="69.7109375" style="2" customWidth="1"/>
-    <col min="13042" max="13071" width="4.42578125" style="2" customWidth="1"/>
-    <col min="13072" max="13294" width="17.140625" style="2"/>
-    <col min="13295" max="13295" width="8" style="2" customWidth="1"/>
-    <col min="13296" max="13296" width="10.85546875" style="2" customWidth="1"/>
-    <col min="13297" max="13297" width="69.7109375" style="2" customWidth="1"/>
-    <col min="13298" max="13327" width="4.42578125" style="2" customWidth="1"/>
-    <col min="13328" max="13550" width="17.140625" style="2"/>
-    <col min="13551" max="13551" width="8" style="2" customWidth="1"/>
-    <col min="13552" max="13552" width="10.85546875" style="2" customWidth="1"/>
-    <col min="13553" max="13553" width="69.7109375" style="2" customWidth="1"/>
-    <col min="13554" max="13583" width="4.42578125" style="2" customWidth="1"/>
-    <col min="13584" max="13806" width="17.140625" style="2"/>
-    <col min="13807" max="13807" width="8" style="2" customWidth="1"/>
-    <col min="13808" max="13808" width="10.85546875" style="2" customWidth="1"/>
-    <col min="13809" max="13809" width="69.7109375" style="2" customWidth="1"/>
-    <col min="13810" max="13839" width="4.42578125" style="2" customWidth="1"/>
-    <col min="13840" max="14062" width="17.140625" style="2"/>
-    <col min="14063" max="14063" width="8" style="2" customWidth="1"/>
-    <col min="14064" max="14064" width="10.85546875" style="2" customWidth="1"/>
-    <col min="14065" max="14065" width="69.7109375" style="2" customWidth="1"/>
-    <col min="14066" max="14095" width="4.42578125" style="2" customWidth="1"/>
-    <col min="14096" max="14318" width="17.140625" style="2"/>
-    <col min="14319" max="14319" width="8" style="2" customWidth="1"/>
-    <col min="14320" max="14320" width="10.85546875" style="2" customWidth="1"/>
-    <col min="14321" max="14321" width="69.7109375" style="2" customWidth="1"/>
-    <col min="14322" max="14351" width="4.42578125" style="2" customWidth="1"/>
-    <col min="14352" max="14574" width="17.140625" style="2"/>
-    <col min="14575" max="14575" width="8" style="2" customWidth="1"/>
-    <col min="14576" max="14576" width="10.85546875" style="2" customWidth="1"/>
-    <col min="14577" max="14577" width="69.7109375" style="2" customWidth="1"/>
-    <col min="14578" max="14607" width="4.42578125" style="2" customWidth="1"/>
-    <col min="14608" max="14830" width="17.140625" style="2"/>
-    <col min="14831" max="14831" width="8" style="2" customWidth="1"/>
-    <col min="14832" max="14832" width="10.85546875" style="2" customWidth="1"/>
-    <col min="14833" max="14833" width="69.7109375" style="2" customWidth="1"/>
-    <col min="14834" max="14863" width="4.42578125" style="2" customWidth="1"/>
-    <col min="14864" max="15086" width="17.140625" style="2"/>
-    <col min="15087" max="15087" width="8" style="2" customWidth="1"/>
-    <col min="15088" max="15088" width="10.85546875" style="2" customWidth="1"/>
-    <col min="15089" max="15089" width="69.7109375" style="2" customWidth="1"/>
-    <col min="15090" max="15119" width="4.42578125" style="2" customWidth="1"/>
-    <col min="15120" max="15342" width="17.140625" style="2"/>
-    <col min="15343" max="15343" width="8" style="2" customWidth="1"/>
-    <col min="15344" max="15344" width="10.85546875" style="2" customWidth="1"/>
-    <col min="15345" max="15345" width="69.7109375" style="2" customWidth="1"/>
-    <col min="15346" max="15375" width="4.42578125" style="2" customWidth="1"/>
-    <col min="15376" max="15598" width="17.140625" style="2"/>
-    <col min="15599" max="15599" width="8" style="2" customWidth="1"/>
-    <col min="15600" max="15600" width="10.85546875" style="2" customWidth="1"/>
-    <col min="15601" max="15601" width="69.7109375" style="2" customWidth="1"/>
-    <col min="15602" max="15631" width="4.42578125" style="2" customWidth="1"/>
-    <col min="15632" max="15854" width="17.140625" style="2"/>
-    <col min="15855" max="15855" width="8" style="2" customWidth="1"/>
-    <col min="15856" max="15856" width="10.85546875" style="2" customWidth="1"/>
-    <col min="15857" max="15857" width="69.7109375" style="2" customWidth="1"/>
-    <col min="15858" max="15887" width="4.42578125" style="2" customWidth="1"/>
-    <col min="15888" max="16110" width="17.140625" style="2"/>
-    <col min="16111" max="16111" width="8" style="2" customWidth="1"/>
-    <col min="16112" max="16112" width="10.85546875" style="2" customWidth="1"/>
-    <col min="16113" max="16113" width="69.7109375" style="2" customWidth="1"/>
-    <col min="16114" max="16143" width="4.42578125" style="2" customWidth="1"/>
-    <col min="16144" max="16384" width="17.140625" style="2"/>
+    <col min="4" max="12" width="4.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.42578125" style="2" customWidth="1"/>
+    <col min="15" max="237" width="17.140625" style="2"/>
+    <col min="238" max="238" width="8" style="2" customWidth="1"/>
+    <col min="239" max="239" width="10.85546875" style="2" customWidth="1"/>
+    <col min="240" max="240" width="69.7109375" style="2" customWidth="1"/>
+    <col min="241" max="270" width="4.42578125" style="2" customWidth="1"/>
+    <col min="271" max="493" width="17.140625" style="2"/>
+    <col min="494" max="494" width="8" style="2" customWidth="1"/>
+    <col min="495" max="495" width="10.85546875" style="2" customWidth="1"/>
+    <col min="496" max="496" width="69.7109375" style="2" customWidth="1"/>
+    <col min="497" max="526" width="4.42578125" style="2" customWidth="1"/>
+    <col min="527" max="749" width="17.140625" style="2"/>
+    <col min="750" max="750" width="8" style="2" customWidth="1"/>
+    <col min="751" max="751" width="10.85546875" style="2" customWidth="1"/>
+    <col min="752" max="752" width="69.7109375" style="2" customWidth="1"/>
+    <col min="753" max="782" width="4.42578125" style="2" customWidth="1"/>
+    <col min="783" max="1005" width="17.140625" style="2"/>
+    <col min="1006" max="1006" width="8" style="2" customWidth="1"/>
+    <col min="1007" max="1007" width="10.85546875" style="2" customWidth="1"/>
+    <col min="1008" max="1008" width="69.7109375" style="2" customWidth="1"/>
+    <col min="1009" max="1038" width="4.42578125" style="2" customWidth="1"/>
+    <col min="1039" max="1261" width="17.140625" style="2"/>
+    <col min="1262" max="1262" width="8" style="2" customWidth="1"/>
+    <col min="1263" max="1263" width="10.85546875" style="2" customWidth="1"/>
+    <col min="1264" max="1264" width="69.7109375" style="2" customWidth="1"/>
+    <col min="1265" max="1294" width="4.42578125" style="2" customWidth="1"/>
+    <col min="1295" max="1517" width="17.140625" style="2"/>
+    <col min="1518" max="1518" width="8" style="2" customWidth="1"/>
+    <col min="1519" max="1519" width="10.85546875" style="2" customWidth="1"/>
+    <col min="1520" max="1520" width="69.7109375" style="2" customWidth="1"/>
+    <col min="1521" max="1550" width="4.42578125" style="2" customWidth="1"/>
+    <col min="1551" max="1773" width="17.140625" style="2"/>
+    <col min="1774" max="1774" width="8" style="2" customWidth="1"/>
+    <col min="1775" max="1775" width="10.85546875" style="2" customWidth="1"/>
+    <col min="1776" max="1776" width="69.7109375" style="2" customWidth="1"/>
+    <col min="1777" max="1806" width="4.42578125" style="2" customWidth="1"/>
+    <col min="1807" max="2029" width="17.140625" style="2"/>
+    <col min="2030" max="2030" width="8" style="2" customWidth="1"/>
+    <col min="2031" max="2031" width="10.85546875" style="2" customWidth="1"/>
+    <col min="2032" max="2032" width="69.7109375" style="2" customWidth="1"/>
+    <col min="2033" max="2062" width="4.42578125" style="2" customWidth="1"/>
+    <col min="2063" max="2285" width="17.140625" style="2"/>
+    <col min="2286" max="2286" width="8" style="2" customWidth="1"/>
+    <col min="2287" max="2287" width="10.85546875" style="2" customWidth="1"/>
+    <col min="2288" max="2288" width="69.7109375" style="2" customWidth="1"/>
+    <col min="2289" max="2318" width="4.42578125" style="2" customWidth="1"/>
+    <col min="2319" max="2541" width="17.140625" style="2"/>
+    <col min="2542" max="2542" width="8" style="2" customWidth="1"/>
+    <col min="2543" max="2543" width="10.85546875" style="2" customWidth="1"/>
+    <col min="2544" max="2544" width="69.7109375" style="2" customWidth="1"/>
+    <col min="2545" max="2574" width="4.42578125" style="2" customWidth="1"/>
+    <col min="2575" max="2797" width="17.140625" style="2"/>
+    <col min="2798" max="2798" width="8" style="2" customWidth="1"/>
+    <col min="2799" max="2799" width="10.85546875" style="2" customWidth="1"/>
+    <col min="2800" max="2800" width="69.7109375" style="2" customWidth="1"/>
+    <col min="2801" max="2830" width="4.42578125" style="2" customWidth="1"/>
+    <col min="2831" max="3053" width="17.140625" style="2"/>
+    <col min="3054" max="3054" width="8" style="2" customWidth="1"/>
+    <col min="3055" max="3055" width="10.85546875" style="2" customWidth="1"/>
+    <col min="3056" max="3056" width="69.7109375" style="2" customWidth="1"/>
+    <col min="3057" max="3086" width="4.42578125" style="2" customWidth="1"/>
+    <col min="3087" max="3309" width="17.140625" style="2"/>
+    <col min="3310" max="3310" width="8" style="2" customWidth="1"/>
+    <col min="3311" max="3311" width="10.85546875" style="2" customWidth="1"/>
+    <col min="3312" max="3312" width="69.7109375" style="2" customWidth="1"/>
+    <col min="3313" max="3342" width="4.42578125" style="2" customWidth="1"/>
+    <col min="3343" max="3565" width="17.140625" style="2"/>
+    <col min="3566" max="3566" width="8" style="2" customWidth="1"/>
+    <col min="3567" max="3567" width="10.85546875" style="2" customWidth="1"/>
+    <col min="3568" max="3568" width="69.7109375" style="2" customWidth="1"/>
+    <col min="3569" max="3598" width="4.42578125" style="2" customWidth="1"/>
+    <col min="3599" max="3821" width="17.140625" style="2"/>
+    <col min="3822" max="3822" width="8" style="2" customWidth="1"/>
+    <col min="3823" max="3823" width="10.85546875" style="2" customWidth="1"/>
+    <col min="3824" max="3824" width="69.7109375" style="2" customWidth="1"/>
+    <col min="3825" max="3854" width="4.42578125" style="2" customWidth="1"/>
+    <col min="3855" max="4077" width="17.140625" style="2"/>
+    <col min="4078" max="4078" width="8" style="2" customWidth="1"/>
+    <col min="4079" max="4079" width="10.85546875" style="2" customWidth="1"/>
+    <col min="4080" max="4080" width="69.7109375" style="2" customWidth="1"/>
+    <col min="4081" max="4110" width="4.42578125" style="2" customWidth="1"/>
+    <col min="4111" max="4333" width="17.140625" style="2"/>
+    <col min="4334" max="4334" width="8" style="2" customWidth="1"/>
+    <col min="4335" max="4335" width="10.85546875" style="2" customWidth="1"/>
+    <col min="4336" max="4336" width="69.7109375" style="2" customWidth="1"/>
+    <col min="4337" max="4366" width="4.42578125" style="2" customWidth="1"/>
+    <col min="4367" max="4589" width="17.140625" style="2"/>
+    <col min="4590" max="4590" width="8" style="2" customWidth="1"/>
+    <col min="4591" max="4591" width="10.85546875" style="2" customWidth="1"/>
+    <col min="4592" max="4592" width="69.7109375" style="2" customWidth="1"/>
+    <col min="4593" max="4622" width="4.42578125" style="2" customWidth="1"/>
+    <col min="4623" max="4845" width="17.140625" style="2"/>
+    <col min="4846" max="4846" width="8" style="2" customWidth="1"/>
+    <col min="4847" max="4847" width="10.85546875" style="2" customWidth="1"/>
+    <col min="4848" max="4848" width="69.7109375" style="2" customWidth="1"/>
+    <col min="4849" max="4878" width="4.42578125" style="2" customWidth="1"/>
+    <col min="4879" max="5101" width="17.140625" style="2"/>
+    <col min="5102" max="5102" width="8" style="2" customWidth="1"/>
+    <col min="5103" max="5103" width="10.85546875" style="2" customWidth="1"/>
+    <col min="5104" max="5104" width="69.7109375" style="2" customWidth="1"/>
+    <col min="5105" max="5134" width="4.42578125" style="2" customWidth="1"/>
+    <col min="5135" max="5357" width="17.140625" style="2"/>
+    <col min="5358" max="5358" width="8" style="2" customWidth="1"/>
+    <col min="5359" max="5359" width="10.85546875" style="2" customWidth="1"/>
+    <col min="5360" max="5360" width="69.7109375" style="2" customWidth="1"/>
+    <col min="5361" max="5390" width="4.42578125" style="2" customWidth="1"/>
+    <col min="5391" max="5613" width="17.140625" style="2"/>
+    <col min="5614" max="5614" width="8" style="2" customWidth="1"/>
+    <col min="5615" max="5615" width="10.85546875" style="2" customWidth="1"/>
+    <col min="5616" max="5616" width="69.7109375" style="2" customWidth="1"/>
+    <col min="5617" max="5646" width="4.42578125" style="2" customWidth="1"/>
+    <col min="5647" max="5869" width="17.140625" style="2"/>
+    <col min="5870" max="5870" width="8" style="2" customWidth="1"/>
+    <col min="5871" max="5871" width="10.85546875" style="2" customWidth="1"/>
+    <col min="5872" max="5872" width="69.7109375" style="2" customWidth="1"/>
+    <col min="5873" max="5902" width="4.42578125" style="2" customWidth="1"/>
+    <col min="5903" max="6125" width="17.140625" style="2"/>
+    <col min="6126" max="6126" width="8" style="2" customWidth="1"/>
+    <col min="6127" max="6127" width="10.85546875" style="2" customWidth="1"/>
+    <col min="6128" max="6128" width="69.7109375" style="2" customWidth="1"/>
+    <col min="6129" max="6158" width="4.42578125" style="2" customWidth="1"/>
+    <col min="6159" max="6381" width="17.140625" style="2"/>
+    <col min="6382" max="6382" width="8" style="2" customWidth="1"/>
+    <col min="6383" max="6383" width="10.85546875" style="2" customWidth="1"/>
+    <col min="6384" max="6384" width="69.7109375" style="2" customWidth="1"/>
+    <col min="6385" max="6414" width="4.42578125" style="2" customWidth="1"/>
+    <col min="6415" max="6637" width="17.140625" style="2"/>
+    <col min="6638" max="6638" width="8" style="2" customWidth="1"/>
+    <col min="6639" max="6639" width="10.85546875" style="2" customWidth="1"/>
+    <col min="6640" max="6640" width="69.7109375" style="2" customWidth="1"/>
+    <col min="6641" max="6670" width="4.42578125" style="2" customWidth="1"/>
+    <col min="6671" max="6893" width="17.140625" style="2"/>
+    <col min="6894" max="6894" width="8" style="2" customWidth="1"/>
+    <col min="6895" max="6895" width="10.85546875" style="2" customWidth="1"/>
+    <col min="6896" max="6896" width="69.7109375" style="2" customWidth="1"/>
+    <col min="6897" max="6926" width="4.42578125" style="2" customWidth="1"/>
+    <col min="6927" max="7149" width="17.140625" style="2"/>
+    <col min="7150" max="7150" width="8" style="2" customWidth="1"/>
+    <col min="7151" max="7151" width="10.85546875" style="2" customWidth="1"/>
+    <col min="7152" max="7152" width="69.7109375" style="2" customWidth="1"/>
+    <col min="7153" max="7182" width="4.42578125" style="2" customWidth="1"/>
+    <col min="7183" max="7405" width="17.140625" style="2"/>
+    <col min="7406" max="7406" width="8" style="2" customWidth="1"/>
+    <col min="7407" max="7407" width="10.85546875" style="2" customWidth="1"/>
+    <col min="7408" max="7408" width="69.7109375" style="2" customWidth="1"/>
+    <col min="7409" max="7438" width="4.42578125" style="2" customWidth="1"/>
+    <col min="7439" max="7661" width="17.140625" style="2"/>
+    <col min="7662" max="7662" width="8" style="2" customWidth="1"/>
+    <col min="7663" max="7663" width="10.85546875" style="2" customWidth="1"/>
+    <col min="7664" max="7664" width="69.7109375" style="2" customWidth="1"/>
+    <col min="7665" max="7694" width="4.42578125" style="2" customWidth="1"/>
+    <col min="7695" max="7917" width="17.140625" style="2"/>
+    <col min="7918" max="7918" width="8" style="2" customWidth="1"/>
+    <col min="7919" max="7919" width="10.85546875" style="2" customWidth="1"/>
+    <col min="7920" max="7920" width="69.7109375" style="2" customWidth="1"/>
+    <col min="7921" max="7950" width="4.42578125" style="2" customWidth="1"/>
+    <col min="7951" max="8173" width="17.140625" style="2"/>
+    <col min="8174" max="8174" width="8" style="2" customWidth="1"/>
+    <col min="8175" max="8175" width="10.85546875" style="2" customWidth="1"/>
+    <col min="8176" max="8176" width="69.7109375" style="2" customWidth="1"/>
+    <col min="8177" max="8206" width="4.42578125" style="2" customWidth="1"/>
+    <col min="8207" max="8429" width="17.140625" style="2"/>
+    <col min="8430" max="8430" width="8" style="2" customWidth="1"/>
+    <col min="8431" max="8431" width="10.85546875" style="2" customWidth="1"/>
+    <col min="8432" max="8432" width="69.7109375" style="2" customWidth="1"/>
+    <col min="8433" max="8462" width="4.42578125" style="2" customWidth="1"/>
+    <col min="8463" max="8685" width="17.140625" style="2"/>
+    <col min="8686" max="8686" width="8" style="2" customWidth="1"/>
+    <col min="8687" max="8687" width="10.85546875" style="2" customWidth="1"/>
+    <col min="8688" max="8688" width="69.7109375" style="2" customWidth="1"/>
+    <col min="8689" max="8718" width="4.42578125" style="2" customWidth="1"/>
+    <col min="8719" max="8941" width="17.140625" style="2"/>
+    <col min="8942" max="8942" width="8" style="2" customWidth="1"/>
+    <col min="8943" max="8943" width="10.85546875" style="2" customWidth="1"/>
+    <col min="8944" max="8944" width="69.7109375" style="2" customWidth="1"/>
+    <col min="8945" max="8974" width="4.42578125" style="2" customWidth="1"/>
+    <col min="8975" max="9197" width="17.140625" style="2"/>
+    <col min="9198" max="9198" width="8" style="2" customWidth="1"/>
+    <col min="9199" max="9199" width="10.85546875" style="2" customWidth="1"/>
+    <col min="9200" max="9200" width="69.7109375" style="2" customWidth="1"/>
+    <col min="9201" max="9230" width="4.42578125" style="2" customWidth="1"/>
+    <col min="9231" max="9453" width="17.140625" style="2"/>
+    <col min="9454" max="9454" width="8" style="2" customWidth="1"/>
+    <col min="9455" max="9455" width="10.85546875" style="2" customWidth="1"/>
+    <col min="9456" max="9456" width="69.7109375" style="2" customWidth="1"/>
+    <col min="9457" max="9486" width="4.42578125" style="2" customWidth="1"/>
+    <col min="9487" max="9709" width="17.140625" style="2"/>
+    <col min="9710" max="9710" width="8" style="2" customWidth="1"/>
+    <col min="9711" max="9711" width="10.85546875" style="2" customWidth="1"/>
+    <col min="9712" max="9712" width="69.7109375" style="2" customWidth="1"/>
+    <col min="9713" max="9742" width="4.42578125" style="2" customWidth="1"/>
+    <col min="9743" max="9965" width="17.140625" style="2"/>
+    <col min="9966" max="9966" width="8" style="2" customWidth="1"/>
+    <col min="9967" max="9967" width="10.85546875" style="2" customWidth="1"/>
+    <col min="9968" max="9968" width="69.7109375" style="2" customWidth="1"/>
+    <col min="9969" max="9998" width="4.42578125" style="2" customWidth="1"/>
+    <col min="9999" max="10221" width="17.140625" style="2"/>
+    <col min="10222" max="10222" width="8" style="2" customWidth="1"/>
+    <col min="10223" max="10223" width="10.85546875" style="2" customWidth="1"/>
+    <col min="10224" max="10224" width="69.7109375" style="2" customWidth="1"/>
+    <col min="10225" max="10254" width="4.42578125" style="2" customWidth="1"/>
+    <col min="10255" max="10477" width="17.140625" style="2"/>
+    <col min="10478" max="10478" width="8" style="2" customWidth="1"/>
+    <col min="10479" max="10479" width="10.85546875" style="2" customWidth="1"/>
+    <col min="10480" max="10480" width="69.7109375" style="2" customWidth="1"/>
+    <col min="10481" max="10510" width="4.42578125" style="2" customWidth="1"/>
+    <col min="10511" max="10733" width="17.140625" style="2"/>
+    <col min="10734" max="10734" width="8" style="2" customWidth="1"/>
+    <col min="10735" max="10735" width="10.85546875" style="2" customWidth="1"/>
+    <col min="10736" max="10736" width="69.7109375" style="2" customWidth="1"/>
+    <col min="10737" max="10766" width="4.42578125" style="2" customWidth="1"/>
+    <col min="10767" max="10989" width="17.140625" style="2"/>
+    <col min="10990" max="10990" width="8" style="2" customWidth="1"/>
+    <col min="10991" max="10991" width="10.85546875" style="2" customWidth="1"/>
+    <col min="10992" max="10992" width="69.7109375" style="2" customWidth="1"/>
+    <col min="10993" max="11022" width="4.42578125" style="2" customWidth="1"/>
+    <col min="11023" max="11245" width="17.140625" style="2"/>
+    <col min="11246" max="11246" width="8" style="2" customWidth="1"/>
+    <col min="11247" max="11247" width="10.85546875" style="2" customWidth="1"/>
+    <col min="11248" max="11248" width="69.7109375" style="2" customWidth="1"/>
+    <col min="11249" max="11278" width="4.42578125" style="2" customWidth="1"/>
+    <col min="11279" max="11501" width="17.140625" style="2"/>
+    <col min="11502" max="11502" width="8" style="2" customWidth="1"/>
+    <col min="11503" max="11503" width="10.85546875" style="2" customWidth="1"/>
+    <col min="11504" max="11504" width="69.7109375" style="2" customWidth="1"/>
+    <col min="11505" max="11534" width="4.42578125" style="2" customWidth="1"/>
+    <col min="11535" max="11757" width="17.140625" style="2"/>
+    <col min="11758" max="11758" width="8" style="2" customWidth="1"/>
+    <col min="11759" max="11759" width="10.85546875" style="2" customWidth="1"/>
+    <col min="11760" max="11760" width="69.7109375" style="2" customWidth="1"/>
+    <col min="11761" max="11790" width="4.42578125" style="2" customWidth="1"/>
+    <col min="11791" max="12013" width="17.140625" style="2"/>
+    <col min="12014" max="12014" width="8" style="2" customWidth="1"/>
+    <col min="12015" max="12015" width="10.85546875" style="2" customWidth="1"/>
+    <col min="12016" max="12016" width="69.7109375" style="2" customWidth="1"/>
+    <col min="12017" max="12046" width="4.42578125" style="2" customWidth="1"/>
+    <col min="12047" max="12269" width="17.140625" style="2"/>
+    <col min="12270" max="12270" width="8" style="2" customWidth="1"/>
+    <col min="12271" max="12271" width="10.85546875" style="2" customWidth="1"/>
+    <col min="12272" max="12272" width="69.7109375" style="2" customWidth="1"/>
+    <col min="12273" max="12302" width="4.42578125" style="2" customWidth="1"/>
+    <col min="12303" max="12525" width="17.140625" style="2"/>
+    <col min="12526" max="12526" width="8" style="2" customWidth="1"/>
+    <col min="12527" max="12527" width="10.85546875" style="2" customWidth="1"/>
+    <col min="12528" max="12528" width="69.7109375" style="2" customWidth="1"/>
+    <col min="12529" max="12558" width="4.42578125" style="2" customWidth="1"/>
+    <col min="12559" max="12781" width="17.140625" style="2"/>
+    <col min="12782" max="12782" width="8" style="2" customWidth="1"/>
+    <col min="12783" max="12783" width="10.85546875" style="2" customWidth="1"/>
+    <col min="12784" max="12784" width="69.7109375" style="2" customWidth="1"/>
+    <col min="12785" max="12814" width="4.42578125" style="2" customWidth="1"/>
+    <col min="12815" max="13037" width="17.140625" style="2"/>
+    <col min="13038" max="13038" width="8" style="2" customWidth="1"/>
+    <col min="13039" max="13039" width="10.85546875" style="2" customWidth="1"/>
+    <col min="13040" max="13040" width="69.7109375" style="2" customWidth="1"/>
+    <col min="13041" max="13070" width="4.42578125" style="2" customWidth="1"/>
+    <col min="13071" max="13293" width="17.140625" style="2"/>
+    <col min="13294" max="13294" width="8" style="2" customWidth="1"/>
+    <col min="13295" max="13295" width="10.85546875" style="2" customWidth="1"/>
+    <col min="13296" max="13296" width="69.7109375" style="2" customWidth="1"/>
+    <col min="13297" max="13326" width="4.42578125" style="2" customWidth="1"/>
+    <col min="13327" max="13549" width="17.140625" style="2"/>
+    <col min="13550" max="13550" width="8" style="2" customWidth="1"/>
+    <col min="13551" max="13551" width="10.85546875" style="2" customWidth="1"/>
+    <col min="13552" max="13552" width="69.7109375" style="2" customWidth="1"/>
+    <col min="13553" max="13582" width="4.42578125" style="2" customWidth="1"/>
+    <col min="13583" max="13805" width="17.140625" style="2"/>
+    <col min="13806" max="13806" width="8" style="2" customWidth="1"/>
+    <col min="13807" max="13807" width="10.85546875" style="2" customWidth="1"/>
+    <col min="13808" max="13808" width="69.7109375" style="2" customWidth="1"/>
+    <col min="13809" max="13838" width="4.42578125" style="2" customWidth="1"/>
+    <col min="13839" max="14061" width="17.140625" style="2"/>
+    <col min="14062" max="14062" width="8" style="2" customWidth="1"/>
+    <col min="14063" max="14063" width="10.85546875" style="2" customWidth="1"/>
+    <col min="14064" max="14064" width="69.7109375" style="2" customWidth="1"/>
+    <col min="14065" max="14094" width="4.42578125" style="2" customWidth="1"/>
+    <col min="14095" max="14317" width="17.140625" style="2"/>
+    <col min="14318" max="14318" width="8" style="2" customWidth="1"/>
+    <col min="14319" max="14319" width="10.85546875" style="2" customWidth="1"/>
+    <col min="14320" max="14320" width="69.7109375" style="2" customWidth="1"/>
+    <col min="14321" max="14350" width="4.42578125" style="2" customWidth="1"/>
+    <col min="14351" max="14573" width="17.140625" style="2"/>
+    <col min="14574" max="14574" width="8" style="2" customWidth="1"/>
+    <col min="14575" max="14575" width="10.85546875" style="2" customWidth="1"/>
+    <col min="14576" max="14576" width="69.7109375" style="2" customWidth="1"/>
+    <col min="14577" max="14606" width="4.42578125" style="2" customWidth="1"/>
+    <col min="14607" max="14829" width="17.140625" style="2"/>
+    <col min="14830" max="14830" width="8" style="2" customWidth="1"/>
+    <col min="14831" max="14831" width="10.85546875" style="2" customWidth="1"/>
+    <col min="14832" max="14832" width="69.7109375" style="2" customWidth="1"/>
+    <col min="14833" max="14862" width="4.42578125" style="2" customWidth="1"/>
+    <col min="14863" max="15085" width="17.140625" style="2"/>
+    <col min="15086" max="15086" width="8" style="2" customWidth="1"/>
+    <col min="15087" max="15087" width="10.85546875" style="2" customWidth="1"/>
+    <col min="15088" max="15088" width="69.7109375" style="2" customWidth="1"/>
+    <col min="15089" max="15118" width="4.42578125" style="2" customWidth="1"/>
+    <col min="15119" max="15341" width="17.140625" style="2"/>
+    <col min="15342" max="15342" width="8" style="2" customWidth="1"/>
+    <col min="15343" max="15343" width="10.85546875" style="2" customWidth="1"/>
+    <col min="15344" max="15344" width="69.7109375" style="2" customWidth="1"/>
+    <col min="15345" max="15374" width="4.42578125" style="2" customWidth="1"/>
+    <col min="15375" max="15597" width="17.140625" style="2"/>
+    <col min="15598" max="15598" width="8" style="2" customWidth="1"/>
+    <col min="15599" max="15599" width="10.85546875" style="2" customWidth="1"/>
+    <col min="15600" max="15600" width="69.7109375" style="2" customWidth="1"/>
+    <col min="15601" max="15630" width="4.42578125" style="2" customWidth="1"/>
+    <col min="15631" max="15853" width="17.140625" style="2"/>
+    <col min="15854" max="15854" width="8" style="2" customWidth="1"/>
+    <col min="15855" max="15855" width="10.85546875" style="2" customWidth="1"/>
+    <col min="15856" max="15856" width="69.7109375" style="2" customWidth="1"/>
+    <col min="15857" max="15886" width="4.42578125" style="2" customWidth="1"/>
+    <col min="15887" max="16109" width="17.140625" style="2"/>
+    <col min="16110" max="16110" width="8" style="2" customWidth="1"/>
+    <col min="16111" max="16111" width="10.85546875" style="2" customWidth="1"/>
+    <col min="16112" max="16112" width="69.7109375" style="2" customWidth="1"/>
+    <col min="16113" max="16142" width="4.42578125" style="2" customWidth="1"/>
+    <col min="16143" max="16384" width="17.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
-      <c r="N1" s="2"/>
-    </row>
-    <row r="3" spans="1:14" ht="24" customHeight="1">
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="17"/>
-    </row>
-    <row r="4" spans="1:14" ht="142.5" customHeight="1">
-      <c r="B4" s="12"/>
-      <c r="C4" s="13" t="s">
-        <v>41</v>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M1" s="2"/>
+    </row>
+    <row r="3" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="15"/>
+    </row>
+    <row r="4" spans="1:13" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="11"/>
+      <c r="C4" s="12" t="s">
+        <v>39</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>31</v>
@@ -1078,10 +1049,10 @@
         <v>34</v>
       </c>
       <c r="H4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>0</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>36</v>
@@ -1093,63 +1064,57 @@
         <v>38</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="N4" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="62.25" customHeight="1">
+    <row r="5" spans="1:13" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
-      <c r="B5" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>43</v>
+      <c r="B5" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="D5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="G5" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="H5" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="I5" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="J5" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="K5" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="L5" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="M5" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="L5" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="B6" s="11" t="s">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
@@ -1159,20 +1124,19 @@
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="9"/>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="B7" s="11" t="s">
+      <c r="M6" s="9"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="D7" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
@@ -1180,122 +1144,116 @@
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="9"/>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="B8" s="11" t="s">
+      <c r="M7" s="9"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="E8" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="9"/>
-    </row>
-    <row r="9" spans="1:14">
-      <c r="B9" s="11" t="s">
+      <c r="M8" s="9"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="E9" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="9"/>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="B10" s="11" t="s">
+      <c r="M9" s="9"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="E10" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="F10" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>44</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="G10" s="8"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="9"/>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="B11" s="11" t="s">
+      <c r="M10" s="9"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="E11" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" s="8"/>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="9"/>
-    </row>
-    <row r="12" spans="1:14">
-      <c r="B12" s="11" t="s">
+      <c r="M11" s="9"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="E12" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" s="8"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="9"/>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="B13" s="11" t="s">
+      <c r="M12" s="9"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -1305,18 +1263,17 @@
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="H13" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" s="8"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="9"/>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="B14" s="11" t="s">
+      <c r="M13" s="9"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -1327,86 +1284,82 @@
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="I14" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" s="8"/>
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="9"/>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="B15" s="11" t="s">
+      <c r="M14" s="9"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="10"/>
+      <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="I15" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J15" s="8"/>
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="9"/>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="B16" s="11" t="s">
+      <c r="M15" s="9"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="10"/>
+      <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="J16" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="K16" s="8"/>
       <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="9"/>
-    </row>
-    <row r="17" spans="2:14">
-      <c r="B17" s="11" t="s">
+      <c r="M16" s="9"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="10"/>
+      <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="M17" s="8"/>
-      <c r="N17" s="9"/>
-    </row>
-    <row r="18" spans="2:14">
-      <c r="B18" s="11" t="s">
+      <c r="K17" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="L17" s="8"/>
+      <c r="M17" s="9"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" s="10" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="10"/>
+      <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
@@ -1414,20 +1367,19 @@
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="N18" s="9"/>
-    </row>
-    <row r="19" spans="2:14">
-      <c r="B19" s="11" t="s">
+      <c r="L18" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="M18" s="9"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="10" t="s">
         <v>15</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="10"/>
+      <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
@@ -1435,38 +1387,36 @@
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="N19" s="9"/>
-    </row>
-    <row r="20" spans="2:14">
-      <c r="B20" s="11" t="s">
+      <c r="L19" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="M19" s="9"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B20" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="E20" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="8"/>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="9" t="s">
-        <v>44</v>
+      <c r="M20" s="9" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D3:N3"/>
+    <mergeCell ref="D3:M3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1474,14 +1424,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -1494,20 +1444,20 @@
     <col min="9" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" ht="15.75" customHeight="1"/>
-    <row r="4" ht="15.75" customHeight="1"/>
+    <row r="2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>